<commit_message>
new version of calculations
</commit_message>
<xml_diff>
--- a/MCC_calculations.xlsx
+++ b/MCC_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chady\Desktop\Data Science\Group-Project-435\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93708AC8-8BDC-4BF6-A884-3766EC480D1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E29A96-3E80-4EBA-BF5A-A10EB94341F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-3765" windowWidth="15990" windowHeight="25440" xr2:uid="{9A46E975-8275-4129-A090-233569A3FF7C}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
   <si>
     <t>true DNA</t>
   </si>
@@ -124,19 +124,57 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>accuracy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -147,7 +185,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -155,13 +193,282 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDAA40B-92B9-426E-9E7E-D6F682741B4D}">
-  <dimension ref="C1:H41"/>
+  <dimension ref="A1:K62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+      <selection activeCell="E38" sqref="E38:E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,108 +863,109 @@
       </c>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
+      <c r="C15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D15">
-        <v>749</v>
-      </c>
-      <c r="E15">
-        <v>28</v>
-      </c>
-      <c r="F15">
-        <v>26</v>
-      </c>
-      <c r="G15">
-        <v>2</v>
+      <c r="D15" s="2">
+        <v>741</v>
+      </c>
+      <c r="E15" s="2">
+        <v>25</v>
+      </c>
+      <c r="F15" s="2">
+        <v>24</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1</v>
       </c>
       <c r="H15">
         <f>SUM(D15:G15)</f>
-        <v>805</v>
+        <v>791</v>
       </c>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+      <c r="C16" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D16">
-        <v>12</v>
-      </c>
-      <c r="E16">
-        <v>23</v>
-      </c>
-      <c r="F16">
-        <v>5</v>
-      </c>
-      <c r="G16">
+      <c r="D16" s="2">
+        <v>17</v>
+      </c>
+      <c r="E16" s="2">
+        <v>25</v>
+      </c>
+      <c r="F16" s="2">
+        <v>2</v>
+      </c>
+      <c r="G16" s="2">
         <v>0</v>
       </c>
       <c r="H16">
         <f t="shared" ref="H16:H18" si="0">SUM(D16:G16)</f>
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+      <c r="C17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="2">
+        <v>18</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2</v>
+      </c>
+      <c r="F17" s="2">
         <v>11</v>
       </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>5</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
+      <c r="G17" s="2">
+        <v>1</v>
       </c>
       <c r="H17">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+      <c r="C18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D18">
-        <v>14</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>3</v>
-      </c>
-      <c r="G18">
+      <c r="D18" s="2">
+        <v>10</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2</v>
+      </c>
+      <c r="G18" s="2">
         <v>0</v>
       </c>
       <c r="H18">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+      <c r="C19" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D19">
@@ -678,259 +986,546 @@
       </c>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="H23" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="24" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+      <c r="C24" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="3">
         <f>D15</f>
-        <v>749</v>
-      </c>
-      <c r="E24">
+        <v>741</v>
+      </c>
+      <c r="E24" s="3">
         <f>E16</f>
-        <v>23</v>
-      </c>
-      <c r="F24">
+        <v>25</v>
+      </c>
+      <c r="F24" s="3">
         <f>F17</f>
-        <v>5</v>
-      </c>
-      <c r="G24">
+        <v>11</v>
+      </c>
+      <c r="G24" s="3">
         <f>G18</f>
         <v>0</v>
       </c>
+      <c r="H24">
+        <f>SUM(D24:G24)</f>
+        <v>777</v>
+      </c>
     </row>
     <row r="25" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+      <c r="C25" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="3">
         <f>SUM(D16:D18)</f>
-        <v>37</v>
-      </c>
-      <c r="E25">
+        <v>45</v>
+      </c>
+      <c r="E25" s="3">
         <f>SUM(E15,E17:E18)</f>
-        <v>29</v>
-      </c>
-      <c r="F25">
+        <v>27</v>
+      </c>
+      <c r="F25" s="3">
         <f>SUM(F18,F15:F16)</f>
-        <v>34</v>
-      </c>
-      <c r="G25">
+        <v>28</v>
+      </c>
+      <c r="G25" s="3">
         <f>SUM(G15:G17)</f>
         <v>2</v>
       </c>
+      <c r="H25">
+        <f t="shared" ref="H25:H27" si="2">SUM(D25:G25)</f>
+        <v>102</v>
+      </c>
     </row>
     <row r="26" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
+      <c r="C26" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="3">
         <f>SUM(E16:G18)</f>
-        <v>37</v>
-      </c>
-      <c r="E26">
+        <v>43</v>
+      </c>
+      <c r="E26" s="3">
         <f>SUM(D17:D18,F17:G18,D15,F15:G15)</f>
-        <v>810</v>
-      </c>
-      <c r="F26">
+        <v>808</v>
+      </c>
+      <c r="F26" s="3">
         <f>SUM(G18,D15:E16,G15,G16,D18:E18)</f>
-        <v>829</v>
-      </c>
-      <c r="G26">
+        <v>819</v>
+      </c>
+      <c r="G26" s="3">
         <f>SUM(D15:F17)</f>
-        <v>859</v>
+        <v>865</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="2"/>
+        <v>2535</v>
       </c>
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
+      <c r="C27" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="3">
         <f>SUM(E15:G15)</f>
-        <v>56</v>
-      </c>
-      <c r="E27">
+        <v>50</v>
+      </c>
+      <c r="E27" s="3">
         <f>SUM(D16,F16:G16)</f>
-        <v>17</v>
-      </c>
-      <c r="F27">
+        <v>19</v>
+      </c>
+      <c r="F27" s="3">
         <f>SUM(G17,E17,D17)</f>
-        <v>11</v>
-      </c>
-      <c r="G27">
+        <v>21</v>
+      </c>
+      <c r="G27" s="3">
         <f>SUM(D18:F18)</f>
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="2"/>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
+      <c r="C28" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="3">
         <f>SUM(D24:D27)</f>
         <v>879</v>
       </c>
-      <c r="E28">
-        <f t="shared" ref="E28:G28" si="2">SUM(E24:E27)</f>
+      <c r="E28" s="3">
+        <f t="shared" ref="E28:G28" si="3">SUM(E24:E27)</f>
         <v>879</v>
       </c>
-      <c r="F28">
-        <f t="shared" si="2"/>
+      <c r="F28" s="3">
+        <f t="shared" si="3"/>
         <v>879</v>
       </c>
-      <c r="G28">
-        <f t="shared" si="2"/>
+      <c r="G28" s="3">
+        <f t="shared" si="3"/>
         <v>879</v>
       </c>
     </row>
     <row r="32" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
+      <c r="C32" s="3"/>
+      <c r="D32" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G32" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C33" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33" s="4">
         <f>D24/(D24 + D25)</f>
-        <v>0.95292620865139954</v>
-      </c>
-      <c r="E33" s="1">
-        <f t="shared" ref="E33:G33" si="3">E24/(E24 + E25)</f>
-        <v>0.44230769230769229</v>
-      </c>
-      <c r="F33" s="1">
-        <f t="shared" si="3"/>
-        <v>0.12820512820512819</v>
-      </c>
-      <c r="G33" s="1">
-        <f t="shared" si="3"/>
+        <v>0.9427480916030534</v>
+      </c>
+      <c r="E33" s="4">
+        <f t="shared" ref="E33:G33" si="4">E24/(E24 + E25)</f>
+        <v>0.48076923076923078</v>
+      </c>
+      <c r="F33" s="4">
+        <f t="shared" si="4"/>
+        <v>0.28205128205128205</v>
+      </c>
+      <c r="G33" s="4">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C34" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34" s="4">
         <f>D26/SUM(D26,D27)</f>
-        <v>0.39784946236559138</v>
-      </c>
-      <c r="E34" s="1">
-        <f t="shared" ref="E34:G34" si="4">E26/SUM(E26,E27)</f>
-        <v>0.97944377267230953</v>
-      </c>
-      <c r="F34" s="1">
-        <f t="shared" si="4"/>
-        <v>0.98690476190476195</v>
-      </c>
-      <c r="G34" s="1">
-        <f t="shared" si="4"/>
-        <v>0.97947548460661349</v>
-      </c>
-    </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
+        <v>0.46236559139784944</v>
+      </c>
+      <c r="E34" s="4">
+        <f t="shared" ref="E34:G34" si="5">E26/SUM(E26,E27)</f>
+        <v>0.97702539298669888</v>
+      </c>
+      <c r="F34" s="4">
+        <f t="shared" si="5"/>
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="G34" s="4">
+        <f t="shared" si="5"/>
+        <v>0.98631698973774229</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C35" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35" s="4">
         <f>(D24+D26)/(SUM(D24:D27))</f>
-        <v>0.89419795221843001</v>
-      </c>
-      <c r="E35" s="1">
-        <f t="shared" ref="E35:G35" si="5">(E24+E26)/(SUM(E24:E27))</f>
+        <v>0.89192263936291238</v>
+      </c>
+      <c r="E35" s="4">
+        <f t="shared" ref="E35:G35" si="6">(E24+E26)/(SUM(E24:E27))</f>
         <v>0.94766780432309439</v>
       </c>
-      <c r="F35" s="1">
-        <f t="shared" si="5"/>
-        <v>0.94880546075085326</v>
-      </c>
-      <c r="G35" s="1">
-        <f t="shared" si="5"/>
-        <v>0.97724687144482369</v>
-      </c>
-    </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+      <c r="F35" s="4">
+        <f t="shared" si="6"/>
+        <v>0.944254835039818</v>
+      </c>
+      <c r="G35" s="4">
+        <f t="shared" si="6"/>
+        <v>0.98407281001137659</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C36" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36" s="4">
         <f>((D24*D26)-(D25*D27))/(SQRT((D24+D27)*(D24+D25)*(D26+D27)*(D26+D25)))</f>
-        <v>0.38856923411229793</v>
-      </c>
-      <c r="E36" s="1">
-        <f t="shared" ref="E36:G36" si="6">((E24*E26)-(E25*E27))/(SQRT((E24+E27)*(E24+E25)*(E26+E27)*(E26+E25)))</f>
-        <v>0.47741938646266779</v>
-      </c>
-      <c r="F36" s="1">
-        <f t="shared" si="6"/>
-        <v>0.17730427076788519</v>
-      </c>
-      <c r="G36" s="1">
-        <f t="shared" si="6"/>
-        <v>-6.904780513901131E-3</v>
-      </c>
-    </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
+        <v>0.41514525795376256</v>
+      </c>
+      <c r="E36" s="4">
+        <f t="shared" ref="E36:G36" si="7">((E24*E26)-(E25*E27))/(SQRT((E24+E27)*(E24+E25)*(E26+E27)*(E26+E25)))</f>
+        <v>0.49528541443260077</v>
+      </c>
+      <c r="F36" s="4">
+        <f t="shared" si="7"/>
+        <v>0.28260186687654881</v>
+      </c>
+      <c r="G36" s="4">
+        <f t="shared" si="7"/>
+        <v>-5.6181880988320949E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C37" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37" s="4">
         <f>D24/(D24 +D27)</f>
-        <v>0.93043478260869561</v>
-      </c>
-      <c r="E37" s="1">
-        <f t="shared" ref="E37:G37" si="7">E24/(E24 +E27)</f>
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="F37" s="1">
-        <f t="shared" si="7"/>
-        <v>0.3125</v>
-      </c>
-      <c r="G37" s="1">
-        <f t="shared" si="7"/>
+        <v>0.93678887484197215</v>
+      </c>
+      <c r="E37" s="4">
+        <f t="shared" ref="E37:G37" si="8">E24/(E24 +E27)</f>
+        <v>0.56818181818181823</v>
+      </c>
+      <c r="F37" s="4">
+        <f t="shared" si="8"/>
+        <v>0.34375</v>
+      </c>
+      <c r="G37" s="4">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C39" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" s="1">
+        <f>H24/D28</f>
+        <v>0.88395904436860073</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C40" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D40" s="4">
         <f>AVERAGE(D36:G36)</f>
-        <v>0.25909702770723747</v>
-      </c>
-    </row>
-    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D41">
+        <v>0.29685358779102</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C41" s="3"/>
+      <c r="D41" s="3">
         <f>(D36 +E36 + F36 +G36)/4</f>
-        <v>0.25909702770723747</v>
-      </c>
+        <v>0.29685358779102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="5"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="9"/>
+    </row>
+    <row r="45" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="20"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="11"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="12"/>
+      <c r="K45" s="13"/>
+    </row>
+    <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="21"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="13"/>
+    </row>
+    <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="21"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="12"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="12"/>
+      <c r="J47" s="12"/>
+      <c r="K47" s="13"/>
+    </row>
+    <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="22"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="16"/>
+      <c r="K48" s="17"/>
+    </row>
+    <row r="49" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="20"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="11"/>
+      <c r="D49" s="12"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="12"/>
+      <c r="J49" s="12"/>
+      <c r="K49" s="13"/>
+    </row>
+    <row r="50" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="21"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="12"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="12"/>
+      <c r="I50" s="12"/>
+      <c r="J50" s="12"/>
+      <c r="K50" s="13"/>
+    </row>
+    <row r="51" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="21"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
+      <c r="H51" s="12"/>
+      <c r="I51" s="12"/>
+      <c r="J51" s="12"/>
+      <c r="K51" s="13"/>
+    </row>
+    <row r="52" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="22"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="15"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
+      <c r="I52" s="16"/>
+      <c r="J52" s="16"/>
+      <c r="K52" s="17"/>
+    </row>
+    <row r="53" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="20"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="11"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="12"/>
+      <c r="I53" s="12"/>
+      <c r="J53" s="12"/>
+      <c r="K53" s="13"/>
+    </row>
+    <row r="54" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="21"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="11"/>
+      <c r="D54" s="12"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12"/>
+      <c r="I54" s="12"/>
+      <c r="J54" s="12"/>
+      <c r="K54" s="13"/>
+    </row>
+    <row r="55" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="21"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="12"/>
+      <c r="K55" s="13"/>
+    </row>
+    <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="22"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="15"/>
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
+      <c r="I56" s="16"/>
+      <c r="J56" s="16"/>
+      <c r="K56" s="17"/>
+    </row>
+    <row r="57" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="20"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="12"/>
+      <c r="K57" s="13"/>
+    </row>
+    <row r="58" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="21"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="12"/>
+      <c r="K58" s="13"/>
+    </row>
+    <row r="59" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="21"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="11"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+      <c r="H59" s="12"/>
+      <c r="I59" s="12"/>
+      <c r="J59" s="12"/>
+      <c r="K59" s="13"/>
+    </row>
+    <row r="60" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="22"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="15"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="16"/>
+      <c r="H60" s="16"/>
+      <c r="I60" s="16"/>
+      <c r="J60" s="16"/>
+      <c r="K60" s="17"/>
+    </row>
+    <row r="61" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="23"/>
+      <c r="B61" s="24"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="12"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="12"/>
+      <c r="J61" s="12"/>
+      <c r="K61" s="13"/>
+    </row>
+    <row r="62" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="25"/>
+      <c r="B62" s="26"/>
+      <c r="C62" s="19"/>
+      <c r="D62" s="16"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="16"/>
+      <c r="H62" s="16"/>
+      <c r="I62" s="16"/>
+      <c r="J62" s="16"/>
+      <c r="K62" s="17"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
done with project fixed mcc
</commit_message>
<xml_diff>
--- a/MCC_calculations.xlsx
+++ b/MCC_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chady\Desktop\Data Science\Group-Project-435\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7EE132-1629-4145-97F0-7D31701062A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5AC145B-B53A-4797-8D6C-89867251D7E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9A46E975-8275-4129-A090-233569A3FF7C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{9A46E975-8275-4129-A090-233569A3FF7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -178,13 +178,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -195,7 +201,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -218,11 +224,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -236,6 +294,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -553,7 +623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABDAA40B-92B9-426E-9E7E-D6F682741B4D}">
   <dimension ref="C1:P49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="M6" sqref="M6:P9"/>
     </sheetView>
   </sheetViews>
@@ -597,7 +667,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="3:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:16" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
         <v>0</v>
       </c>
@@ -624,84 +694,84 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>4</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="M6" s="2">
-        <v>130</v>
-      </c>
-      <c r="N6" s="2">
-        <v>33</v>
-      </c>
-      <c r="O6" s="2">
-        <v>4</v>
-      </c>
-      <c r="P6" s="2">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="M6" s="6">
+        <v>27</v>
+      </c>
+      <c r="N6" s="7">
+        <v>20</v>
+      </c>
+      <c r="O6" s="7">
+        <v>0</v>
+      </c>
+      <c r="P6" s="7">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="7" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="M7" s="2">
-        <v>38</v>
-      </c>
-      <c r="N7" s="2">
-        <v>278</v>
-      </c>
-      <c r="O7" s="2">
+      <c r="M7" s="8">
+        <v>21</v>
+      </c>
+      <c r="N7" s="9">
+        <v>207</v>
+      </c>
+      <c r="O7" s="9">
         <v>1</v>
       </c>
-      <c r="P7" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="P7" s="9">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="8" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="M8" s="2">
-        <v>5</v>
-      </c>
-      <c r="N8" s="2">
-        <v>3</v>
-      </c>
-      <c r="O8" s="2">
+      <c r="M8" s="8">
+        <v>0</v>
+      </c>
+      <c r="N8" s="9">
         <v>2</v>
       </c>
-      <c r="P8" s="2">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="O8" s="9">
+        <v>1</v>
+      </c>
+      <c r="P8" s="9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>7</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="M9" s="2">
-        <v>218</v>
-      </c>
-      <c r="N9" s="2">
-        <v>209</v>
-      </c>
-      <c r="O9" s="2">
-        <v>15</v>
-      </c>
-      <c r="P9" s="2">
-        <v>7504</v>
+      <c r="M9" s="8">
+        <v>36</v>
+      </c>
+      <c r="N9" s="9">
+        <v>71</v>
+      </c>
+      <c r="O9" s="9">
+        <v>1</v>
+      </c>
+      <c r="P9" s="9">
+        <v>7751</v>
       </c>
     </row>
     <row r="10" spans="3:16" x14ac:dyDescent="0.25">
@@ -710,19 +780,19 @@
       </c>
       <c r="M10">
         <f>SUM(M6:M9)</f>
-        <v>391</v>
+        <v>84</v>
       </c>
       <c r="N10">
         <f t="shared" ref="N10:P10" si="0">SUM(N6:N9)</f>
-        <v>523</v>
+        <v>300</v>
       </c>
       <c r="O10">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="P10">
         <f t="shared" si="0"/>
-        <v>7859</v>
+        <v>8408</v>
       </c>
     </row>
     <row r="14" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -749,23 +819,23 @@
       </c>
       <c r="D15" s="5">
         <f>P9</f>
-        <v>7504</v>
+        <v>7751</v>
       </c>
       <c r="E15" s="5">
         <f>N9</f>
-        <v>209</v>
+        <v>71</v>
       </c>
       <c r="F15" s="5">
         <f>M9</f>
-        <v>218</v>
+        <v>36</v>
       </c>
       <c r="G15" s="5">
         <f>O9</f>
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="H15">
         <f>SUM(D15:G15)</f>
-        <v>7946</v>
+        <v>7859</v>
       </c>
       <c r="I15">
         <f>SUM(H15:H18)</f>
@@ -778,15 +848,15 @@
       </c>
       <c r="D16" s="5">
         <f>P7</f>
-        <v>100</v>
+        <v>294</v>
       </c>
       <c r="E16" s="5">
         <f>N7</f>
-        <v>278</v>
+        <v>207</v>
       </c>
       <c r="F16" s="5">
         <f>M7</f>
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="G16" s="5">
         <f>O7</f>
@@ -794,7 +864,7 @@
       </c>
       <c r="H16">
         <f t="shared" ref="H16:H18" si="1">SUM(D16:G16)</f>
-        <v>417</v>
+        <v>523</v>
       </c>
     </row>
     <row r="17" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -803,23 +873,23 @@
       </c>
       <c r="D17" s="5">
         <f>P6</f>
-        <v>234</v>
+        <v>344</v>
       </c>
       <c r="E17" s="5">
         <f>N6</f>
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="F17" s="5">
         <f>M6</f>
-        <v>130</v>
+        <v>27</v>
       </c>
       <c r="G17" s="5">
         <f>O6</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H17">
         <f t="shared" si="1"/>
-        <v>401</v>
+        <v>391</v>
       </c>
     </row>
     <row r="18" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -828,23 +898,23 @@
       </c>
       <c r="D18" s="5">
         <f>P8</f>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E18" s="5">
         <f>N8</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" s="5">
         <f>M8</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G18" s="5">
         <f>O8</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H18">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="3:16" x14ac:dyDescent="0.25">
@@ -853,19 +923,19 @@
       </c>
       <c r="D19">
         <f>SUM(D15:D18)</f>
-        <v>7859</v>
+        <v>8408</v>
       </c>
       <c r="E19">
         <f t="shared" ref="E19:G19" si="2">SUM(E15:E18)</f>
-        <v>523</v>
+        <v>300</v>
       </c>
       <c r="F19">
         <f t="shared" si="2"/>
-        <v>391</v>
+        <v>84</v>
       </c>
       <c r="G19">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="H19">
         <f>SUM(D19:G19)</f>
@@ -896,23 +966,23 @@
       </c>
       <c r="D24" s="3">
         <f>D15</f>
-        <v>7504</v>
+        <v>7751</v>
       </c>
       <c r="E24" s="3">
         <f>E16</f>
-        <v>278</v>
+        <v>207</v>
       </c>
       <c r="F24" s="3">
         <f>F17</f>
-        <v>130</v>
+        <v>27</v>
       </c>
       <c r="G24" s="3">
         <f>G18</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H24">
         <f>SUM(D24:G24)</f>
-        <v>7914</v>
+        <v>7986</v>
       </c>
     </row>
     <row r="25" spans="3:16" x14ac:dyDescent="0.25">
@@ -921,23 +991,23 @@
       </c>
       <c r="D25" s="3">
         <f>SUM(D16:D18)</f>
-        <v>355</v>
+        <v>657</v>
       </c>
       <c r="E25" s="3">
         <f>SUM(E15,E17:E18)</f>
-        <v>245</v>
+        <v>93</v>
       </c>
       <c r="F25" s="3">
         <f>SUM(F18,F15:F16)</f>
-        <v>261</v>
+        <v>57</v>
       </c>
       <c r="G25" s="3">
         <f>SUM(G15:G17)</f>
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="H25">
         <f t="shared" ref="H25:H27" si="3">SUM(D25:G25)</f>
-        <v>881</v>
+        <v>809</v>
       </c>
     </row>
     <row r="26" spans="3:16" x14ac:dyDescent="0.25">
@@ -946,23 +1016,23 @@
       </c>
       <c r="D26" s="3">
         <f>SUM(E16:G18)</f>
-        <v>494</v>
+        <v>279</v>
       </c>
       <c r="E26" s="3">
         <f>SUM(D17:D18,F17:G18,D15,F15:G15)</f>
-        <v>8133</v>
+        <v>8179</v>
       </c>
       <c r="F26" s="3">
         <f>SUM(G18,D15:E16,G15,G16,D18:E18)</f>
-        <v>8133</v>
+        <v>8347</v>
       </c>
       <c r="G26" s="3">
         <f>SUM(D15:F17)</f>
-        <v>8744</v>
+        <v>8771</v>
       </c>
       <c r="H26">
         <f t="shared" si="3"/>
-        <v>25504</v>
+        <v>25576</v>
       </c>
     </row>
     <row r="27" spans="3:16" x14ac:dyDescent="0.25">
@@ -971,23 +1041,23 @@
       </c>
       <c r="D27" s="3">
         <f>SUM(E15:G15)</f>
-        <v>442</v>
+        <v>108</v>
       </c>
       <c r="E27" s="3">
         <f>SUM(D16,F16:G16)</f>
-        <v>139</v>
+        <v>316</v>
       </c>
       <c r="F27" s="3">
         <f>SUM(G17,E17,D17)</f>
-        <v>271</v>
+        <v>364</v>
       </c>
       <c r="G27" s="3">
         <f>SUM(D18:F18)</f>
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H27">
         <f t="shared" si="3"/>
-        <v>881</v>
+        <v>809</v>
       </c>
     </row>
     <row r="28" spans="3:16" x14ac:dyDescent="0.25">
@@ -1044,19 +1114,19 @@
       </c>
       <c r="M32" s="1">
         <f>(M45/(M45+M46))</f>
-        <v>0.95482885863341393</v>
+        <v>0.92186013320646998</v>
       </c>
       <c r="N32" s="1">
         <f t="shared" ref="N32:P32" si="5">(N45/(N45+N46))</f>
-        <v>0.53154875717017214</v>
+        <v>0.69</v>
       </c>
       <c r="O32" s="1">
         <f t="shared" si="5"/>
-        <v>0.33248081841432225</v>
+        <v>0.32142857142857145</v>
       </c>
       <c r="P32" s="1">
         <f t="shared" si="5"/>
-        <v>9.0909090909090912E-2</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="33" spans="3:16" x14ac:dyDescent="0.25">
@@ -1065,38 +1135,38 @@
       </c>
       <c r="D33" s="4">
         <f>D24/(D24 + D25)</f>
-        <v>0.95482885863341393</v>
+        <v>0.92186013320646998</v>
       </c>
       <c r="E33" s="4">
         <f t="shared" ref="E33:G33" si="6">E24/(E24 + E25)</f>
-        <v>0.53154875717017214</v>
+        <v>0.69</v>
       </c>
       <c r="F33" s="4">
         <f t="shared" si="6"/>
-        <v>0.33248081841432225</v>
+        <v>0.32142857142857145</v>
       </c>
       <c r="G33" s="4">
         <f t="shared" si="6"/>
-        <v>9.0909090909090912E-2</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="L33" t="s">
         <v>36</v>
       </c>
       <c r="M33" s="1">
         <f>M47/(M47+M48)</f>
-        <v>0.52777777777777779</v>
+        <v>0.72093023255813948</v>
       </c>
       <c r="N33" s="1">
         <f t="shared" ref="N33:P33" si="7">N47/(N47+N48)</f>
-        <v>0.98319632495164411</v>
+        <v>0.96280164802825197</v>
       </c>
       <c r="O33" s="1">
         <f t="shared" si="7"/>
-        <v>0.96775345073774388</v>
+        <v>0.95821375272643783</v>
       </c>
       <c r="P33" s="1">
         <f t="shared" si="7"/>
-        <v>0.99669440328279946</v>
+        <v>0.99761146496815289</v>
       </c>
     </row>
     <row r="34" spans="3:16" x14ac:dyDescent="0.25">
@@ -1105,38 +1175,38 @@
       </c>
       <c r="D34" s="4">
         <f>D26/SUM(D26,D27)</f>
-        <v>0.52777777777777779</v>
+        <v>0.72093023255813948</v>
       </c>
       <c r="E34" s="4">
         <f t="shared" ref="E34:G34" si="8">E26/SUM(E26,E27)</f>
-        <v>0.98319632495164411</v>
+        <v>0.96280164802825197</v>
       </c>
       <c r="F34" s="4">
         <f t="shared" si="8"/>
-        <v>0.96775345073774388</v>
+        <v>0.95821375272643783</v>
       </c>
       <c r="G34" s="4">
         <f t="shared" si="8"/>
-        <v>0.99669440328279946</v>
+        <v>0.99761146496815289</v>
       </c>
       <c r="L34" t="s">
         <v>37</v>
       </c>
       <c r="M34" s="1">
         <f>(M45+M47)/(SUM(M45:M48))</f>
-        <v>0.90938032973280269</v>
+        <v>0.91301876065946563</v>
       </c>
       <c r="N34" s="1">
         <f t="shared" ref="N34:P34" si="9">(N45+N47)/(SUM(N45:N48))</f>
-        <v>0.95633882888004551</v>
+        <v>0.95349630471859015</v>
       </c>
       <c r="O34" s="1">
         <f t="shared" si="9"/>
-        <v>0.93951108584422971</v>
+        <v>0.95213189312109148</v>
       </c>
       <c r="P34" s="1">
         <f t="shared" si="9"/>
-        <v>0.99442865264354752</v>
+        <v>0.99738487777146101</v>
       </c>
     </row>
     <row r="35" spans="3:16" x14ac:dyDescent="0.25">
@@ -1145,38 +1215,38 @@
       </c>
       <c r="D35" s="4">
         <f>(D24+D26)/(SUM(D24:D27))</f>
-        <v>0.90938032973280269</v>
+        <v>0.91301876065946563</v>
       </c>
       <c r="E35" s="4">
         <f t="shared" ref="E35:G35" si="10">(E24+E26)/(SUM(E24:E27))</f>
-        <v>0.95633882888004551</v>
+        <v>0.95349630471859015</v>
       </c>
       <c r="F35" s="4">
         <f t="shared" si="10"/>
-        <v>0.93951108584422971</v>
+        <v>0.95213189312109148</v>
       </c>
       <c r="G35" s="4">
         <f t="shared" si="10"/>
-        <v>0.99442865264354752</v>
+        <v>0.99738487777146101</v>
       </c>
       <c r="L35" t="s">
         <v>26</v>
       </c>
       <c r="M35" s="1">
         <f>(M45*M47 - M48*M46)/SQRT((M45+M48)*(M45+M46)*(M47+M48)*(M47+M46))</f>
-        <v>0.50394916848041149</v>
+        <v>0.42751329399250115</v>
       </c>
       <c r="N35" s="1">
         <f t="shared" ref="N35:P35" si="11">(N45*N47 - N48*N46)/SQRT((N45+N48)*(N45+N46)*(N47+N48)*(N47+N46))</f>
-        <v>0.57280936252324588</v>
+        <v>0.50103429516958586</v>
       </c>
       <c r="O35" s="1">
         <f t="shared" si="11"/>
-        <v>0.29664360718977767</v>
+        <v>0.13196086458420928</v>
       </c>
       <c r="P35" s="1">
         <f t="shared" si="11"/>
-        <v>7.3837129166254123E-2</v>
+        <v>0.12234173109681386</v>
       </c>
     </row>
     <row r="36" spans="3:16" x14ac:dyDescent="0.25">
@@ -1185,38 +1255,38 @@
       </c>
       <c r="D36" s="4">
         <f>((D24*D26)-(D25*D27))/(SQRT((D24+D27)*(D24+D25)*(D26+D27)*(D26+D25)))</f>
-        <v>0.50394916848041149</v>
+        <v>0.42751329399250115</v>
       </c>
       <c r="E36" s="4">
         <f t="shared" ref="E36:G36" si="12">((E24*E26)-(E25*E27))/(SQRT((E24+E27)*(E24+E25)*(E26+E27)*(E26+E25)))</f>
-        <v>0.57280936252324588</v>
+        <v>0.50103429516958586</v>
       </c>
       <c r="F36" s="4">
         <f t="shared" si="12"/>
-        <v>0.29664360718977767</v>
+        <v>0.13196086458420928</v>
       </c>
       <c r="G36" s="4">
         <f t="shared" si="12"/>
-        <v>7.3837129166254123E-2</v>
+        <v>0.12234173109681386</v>
       </c>
       <c r="L36" t="s">
         <v>38</v>
       </c>
       <c r="M36" s="1">
         <f>M45/(M45+M48)</f>
-        <v>0.94437452806443489</v>
+        <v>0.98625779361241883</v>
       </c>
       <c r="N36" s="1">
         <f t="shared" ref="N36:P36" si="13">N45/(N45+N48)</f>
-        <v>0.66666666666666663</v>
+        <v>0.39579349904397704</v>
       </c>
       <c r="O36" s="1">
         <f t="shared" si="13"/>
-        <v>0.32418952618453867</v>
+        <v>6.9053708439897693E-2</v>
       </c>
       <c r="P36" s="1">
         <f t="shared" si="13"/>
-        <v>6.4516129032258063E-2</v>
+        <v>4.5454545454545456E-2</v>
       </c>
     </row>
     <row r="37" spans="3:16" x14ac:dyDescent="0.25">
@@ -1225,19 +1295,19 @@
       </c>
       <c r="D37" s="4">
         <f>D24/(D24 +D27)</f>
-        <v>0.94437452806443489</v>
+        <v>0.98625779361241883</v>
       </c>
       <c r="E37" s="4">
         <f t="shared" ref="E37:G37" si="14">E24/(E24 +E27)</f>
-        <v>0.66666666666666663</v>
+        <v>0.39579349904397704</v>
       </c>
       <c r="F37" s="4">
         <f t="shared" si="14"/>
-        <v>0.32418952618453867</v>
+        <v>6.9053708439897693E-2</v>
       </c>
       <c r="G37" s="4">
         <f t="shared" si="14"/>
-        <v>6.4516129032258063E-2</v>
+        <v>4.5454545454545456E-2</v>
       </c>
     </row>
     <row r="38" spans="3:16" x14ac:dyDescent="0.25">
@@ -1246,7 +1316,7 @@
       </c>
       <c r="M38">
         <f>AVERAGE(M35:P35)</f>
-        <v>0.36180981683992225</v>
+        <v>0.29571254621077753</v>
       </c>
     </row>
     <row r="39" spans="3:16" x14ac:dyDescent="0.25">
@@ -1255,14 +1325,14 @@
       </c>
       <c r="D39" s="1">
         <f>H24/D28</f>
-        <v>0.89982944855031266</v>
+        <v>0.90801591813530413</v>
       </c>
       <c r="L39" t="s">
         <v>39</v>
       </c>
       <c r="M39" s="1">
         <f>SUM(M45:P45)/SUM(H19)</f>
-        <v>0.89982944855031266</v>
+        <v>0.90801591813530413</v>
       </c>
     </row>
     <row r="40" spans="3:16" x14ac:dyDescent="0.25">
@@ -1271,14 +1341,14 @@
       </c>
       <c r="D40" s="4">
         <f>AVERAGE(D36:G36)</f>
-        <v>0.36180981683992225</v>
+        <v>0.29571254621077753</v>
       </c>
     </row>
     <row r="41" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C41" s="3"/>
       <c r="D41" s="3">
         <f>(D36 +E36 + F36 +G36)/4</f>
-        <v>0.36180981683992225</v>
+        <v>0.29571254621077753</v>
       </c>
     </row>
     <row r="44" spans="3:16" x14ac:dyDescent="0.25">
@@ -1336,19 +1406,19 @@
       </c>
       <c r="M45">
         <f>D15</f>
-        <v>7504</v>
+        <v>7751</v>
       </c>
       <c r="N45">
         <f>E16</f>
-        <v>278</v>
+        <v>207</v>
       </c>
       <c r="O45">
         <f>F17</f>
-        <v>130</v>
+        <v>27</v>
       </c>
       <c r="P45">
         <f>G18</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="3:16" x14ac:dyDescent="0.25">
@@ -1376,19 +1446,19 @@
       </c>
       <c r="M46">
         <f>SUM(D16:D18)</f>
-        <v>355</v>
+        <v>657</v>
       </c>
       <c r="N46">
         <f>SUM(E15,E17:E18)</f>
-        <v>245</v>
+        <v>93</v>
       </c>
       <c r="O46">
         <f>SUM(F15:F16,F18)</f>
-        <v>261</v>
+        <v>57</v>
       </c>
       <c r="P46">
         <f>SUM(G15:G17)</f>
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="3:16" x14ac:dyDescent="0.25">
@@ -1416,19 +1486,19 @@
       </c>
       <c r="M47">
         <f>SUM(E16:G18)</f>
-        <v>494</v>
+        <v>279</v>
       </c>
       <c r="N47">
         <f>SUM(F17:G18,D17:D18,D15,F15:G15)</f>
-        <v>8133</v>
+        <v>8179</v>
       </c>
       <c r="O47">
         <f>SUM(G15:G16,D15:E16,D18:E18,G18)</f>
-        <v>8133</v>
+        <v>8347</v>
       </c>
       <c r="P47">
         <f>SUM(D15:F17)</f>
-        <v>8744</v>
+        <v>8771</v>
       </c>
     </row>
     <row r="48" spans="3:16" x14ac:dyDescent="0.25">
@@ -1456,19 +1526,19 @@
       </c>
       <c r="M48">
         <f>SUM(E15:G15)</f>
-        <v>442</v>
+        <v>108</v>
       </c>
       <c r="N48">
         <f>SUM(D16,F16:G16)</f>
-        <v>139</v>
+        <v>316</v>
       </c>
       <c r="O48">
         <f>SUM(G17,D17:E17)</f>
-        <v>271</v>
+        <v>364</v>
       </c>
       <c r="P48">
         <f>SUM(D18:F18)</f>
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="49" spans="3:7" x14ac:dyDescent="0.25">

</xml_diff>